<commit_message>
dealing with google search HTTPError - too many requests
</commit_message>
<xml_diff>
--- a/mttpJobSearch.xlsx
+++ b/mttpJobSearch.xlsx
@@ -413,47 +413,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>company</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>job title</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>area</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>link</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>term used</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
working on adding more sites to be scraped
</commit_message>
<xml_diff>
--- a/mttpJobSearch.xlsx
+++ b/mttpJobSearch.xlsx
@@ -8,6 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="LinkedIn" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Wellfound" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Others" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -456,4 +458,106 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>company</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>job title</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>area</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>link</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>term used</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>company</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>job title</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>area</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>link</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>term used</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
messing around messing around
</commit_message>
<xml_diff>
--- a/mttpJobSearch.xlsx
+++ b/mttpJobSearch.xlsx
@@ -18,7 +18,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -48,8 +50,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -415,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,6 +455,276 @@
       <c r="F1" t="inlineStr">
         <is>
           <t>term used</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>45092</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Optum </t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Business Development Consultant (EHR Services) - Remote</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Franklin, Tennessee, United States</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/business-development-consultant-ehr-services-remote-at-optum-3637581437</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>pharmacy ehr manager</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>45092</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4 Healing Center </t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Billing Specialist</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Murray, Utah, United States</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/billing-specialist-at-4-healing-center-3637510897?refId=zUHvkrwS6bcg3flBXyE00w%3D%3D&amp;trackingId=bt71DNAtq%2B7kHr3jn%2Fj5Gw%3D%3D&amp;position=15&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>pharmacy ehr manager</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>45092</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4 Healing Center </t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Billing Specialist</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Murray, Utah, United States</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/billing-specialist-at-4-healing-center-3637510897?refId=zUHvkrwS6bcg3flBXyE00w%3D%3D&amp;trackingId=bt71DNAtq%2B7kHr3jn%2Fj5Gw%3D%3D&amp;position=15&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>pharmacy ehr manager</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>45092</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Optum </t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Business Development Consultant (EHR Services) - Remote</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Franklin, Tennessee, United States</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/business-development-consultant-ehr-services-remote-at-optum-3637581437</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>pharmacy ehr specialist</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>45092</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4 Healing Center </t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Billing Specialist</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Murray, Utah, United States</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/billing-specialist-at-4-healing-center-3637510897?refId=zUHvkrwS6bcg3flBXyE00w%3D%3D&amp;trackingId=bt71DNAtq%2B7kHr3jn%2Fj5Gw%3D%3D&amp;position=15&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>pharmacy ehr specialist</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>45092</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4 Healing Center </t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Billing Specialist</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Murray, Utah, United States</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/billing-specialist-at-4-healing-center-3637510897?refId=zUHvkrwS6bcg3flBXyE00w%3D%3D&amp;trackingId=bt71DNAtq%2B7kHr3jn%2Fj5Gw%3D%3D&amp;position=15&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>pharmacy ehr specialist</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>45092</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Optum </t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Business Development Consultant (EHR Services) - Remote</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Franklin, Tennessee, United States</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/business-development-consultant-ehr-services-remote-at-optum-3637581437</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>pharmacy ehr associate</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>45092</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4 Healing Center </t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Billing Specialist</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Murray, Utah, United States</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/billing-specialist-at-4-healing-center-3637510897?refId=zUHvkrwS6bcg3flBXyE00w%3D%3D&amp;trackingId=bt71DNAtq%2B7kHr3jn%2Fj5Gw%3D%3D&amp;position=15&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>pharmacy ehr associate</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>45092</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4 Healing Center </t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Billing Specialist</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Murray, Utah, United States</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/billing-specialist-at-4-healing-center-3637510897?refId=zUHvkrwS6bcg3flBXyE00w%3D%3D&amp;trackingId=bt71DNAtq%2B7kHr3jn%2Fj5Gw%3D%3D&amp;position=15&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>pharmacy ehr associate</t>
         </is>
       </c>
     </row>
@@ -517,7 +790,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -557,6 +830,96 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>45092</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>https://au.linkedin.com/jobs/view/clinical-coder-admin-off-lvl-3-4-5-or-mra-incremental-fairfield-hospital-casual-at-i-work-for-nsw-3629284842</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>pharmacy emr manager</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>45092</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://au.linkedin.com/jobs/view/clinical-coder-admin-off-lvl-3-4-5-or-mra-incremental-fairfield-hospital-casual-at-i-work-for-nsw-3629284842</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>pharmacy emr specialist</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>45092</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>https://au.linkedin.com/jobs/view/clinical-coder-admin-off-lvl-3-4-5-or-mra-incremental-fairfield-hospital-casual-at-i-work-for-nsw-3629284842</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>pharmacy emr associate</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>